<commit_message>
Added missing host species information
</commit_message>
<xml_diff>
--- a/tabular/core/hepadna-ncbi-refseqs-side-data.xlsx
+++ b/tabular/core/hepadna-ncbi-refseqs-side-data.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNArt/Hepadnaviridae-GLUE/tabular/core/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6A1719A-DE29-F140-BE02-5F754ED8406C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10340" yWindow="0" windowWidth="17340" windowHeight="14460" tabRatio="500"/>
+    <workbookView xWindow="10340" yWindow="460" windowWidth="17340" windowHeight="14460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$45</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="215">
   <si>
     <t>DHBV</t>
   </si>
@@ -303,9 +309,6 @@
     <t>African cichlid hepadnavirus</t>
   </si>
   <si>
-    <t>Ground squirrel</t>
-  </si>
-  <si>
     <t>Homo sapiens</t>
   </si>
   <si>
@@ -658,12 +661,24 @@
   </si>
   <si>
     <t>MH158727</t>
+  </si>
+  <si>
+    <t>Anas platyrhynchos</t>
+  </si>
+  <si>
+    <t>Domestic duck</t>
+  </si>
+  <si>
+    <t>Spermophilus beecheyi</t>
+  </si>
+  <si>
+    <t>California ground squirrel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2238,14 +2253,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D12" sqref="A1:H46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.1640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" style="2" customWidth="1"/>
@@ -2257,24 +2272,24 @@
     <col min="9" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>70</v>
@@ -2283,7 +2298,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>38</v>
       </c>
@@ -2294,14 +2309,20 @@
         <v>1</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="G2" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>40</v>
       </c>
@@ -2312,7 +2333,7 @@
         <v>3</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>11</v>
@@ -2325,7 +2346,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>46</v>
       </c>
@@ -2336,7 +2357,7 @@
         <v>19</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>11</v>
@@ -2349,7 +2370,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>43</v>
       </c>
@@ -2360,7 +2381,7 @@
         <v>12</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>11</v>
@@ -2373,7 +2394,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>45</v>
       </c>
@@ -2384,7 +2405,7 @@
         <v>16</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>11</v>
@@ -2397,7 +2418,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>44</v>
       </c>
@@ -2408,20 +2429,20 @@
         <v>15</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>55</v>
       </c>
@@ -2432,7 +2453,7 @@
         <v>34</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>11</v>
@@ -2445,7 +2466,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>56</v>
       </c>
@@ -2456,7 +2477,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>11</v>
@@ -2469,7 +2490,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>58</v>
       </c>
@@ -2480,7 +2501,7 @@
         <v>60</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>11</v>
@@ -2493,7 +2514,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>62</v>
       </c>
@@ -2504,7 +2525,7 @@
         <v>64</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>11</v>
@@ -2517,7 +2538,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>54</v>
       </c>
@@ -2528,10 +2549,10 @@
         <v>33</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F12" s="10"/>
       <c r="G12" s="2" t="s">
@@ -2541,55 +2562,55 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="E13" s="10" t="s">
         <v>116</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>210</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>117</v>
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="H13" s="2" t="s">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="15" t="s">
-        <v>120</v>
-      </c>
       <c r="B14" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F14" s="10"/>
       <c r="G14" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="H14" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>53</v>
       </c>
@@ -2600,10 +2621,10 @@
         <v>32</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="2" t="s">
@@ -2613,261 +2634,261 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="B16" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="B16" s="13" t="s">
-        <v>191</v>
-      </c>
       <c r="C16" s="13" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>123</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>172</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>210</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>124</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="H17" s="2" t="s">
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="15" t="s">
-        <v>127</v>
-      </c>
       <c r="B18" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="H18" s="2" t="s">
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="15" t="s">
-        <v>130</v>
-      </c>
       <c r="B19" s="15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="H19" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="H19" s="2" t="s">
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="15" t="s">
-        <v>133</v>
-      </c>
       <c r="B20" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E20" s="12" t="s">
         <v>66</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G20" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="H20" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="H20" s="2" t="s">
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="15" t="s">
-        <v>136</v>
-      </c>
       <c r="B21" s="15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E21" s="12" t="s">
         <v>66</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G21" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H21" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="H21" s="2" t="s">
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="15" t="s">
-        <v>139</v>
-      </c>
       <c r="B22" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E22" s="12" t="s">
         <v>66</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G22" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="H22" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="H22" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E23" s="12" t="s">
         <v>66</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G23" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="H23" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="H23" s="2" t="s">
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="15" t="s">
-        <v>143</v>
-      </c>
       <c r="B24" s="15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E24" s="12" t="s">
         <v>66</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G24" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="H24" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="H24" s="2" t="s">
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="15" t="s">
-        <v>146</v>
-      </c>
       <c r="B25" s="15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E25" s="12" t="s">
         <v>66</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G25" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="H25" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="H25" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B26" s="15" t="s">
         <v>67</v>
@@ -2876,13 +2897,13 @@
         <v>92</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E26" s="12" t="s">
         <v>66</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>69</v>
@@ -2891,163 +2912,163 @@
         <v>68</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E27" s="12" t="s">
         <v>66</v>
       </c>
       <c r="F27" s="16" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G27" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="H27" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="15" t="s">
-        <v>151</v>
-      </c>
       <c r="B28" s="15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E28" s="12" t="s">
         <v>66</v>
       </c>
       <c r="F28" s="16" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E29" s="12" t="s">
         <v>66</v>
       </c>
       <c r="F29" s="16" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G29" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="H29" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="H29" s="2" t="s">
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="15" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="15" t="s">
-        <v>155</v>
-      </c>
       <c r="B30" s="15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E30" s="12" t="s">
         <v>66</v>
       </c>
       <c r="F30" s="16" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G30" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="H30" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="H30" s="2" t="s">
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="15" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="15" t="s">
-        <v>158</v>
-      </c>
       <c r="B31" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E31" s="12" t="s">
         <v>66</v>
       </c>
       <c r="F31" s="16" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G31" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="H31" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="H31" s="2" t="s">
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="15" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="A32" s="15" t="s">
-        <v>161</v>
-      </c>
       <c r="B32" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E32" s="12" t="s">
         <v>66</v>
       </c>
       <c r="F32" s="16" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G32" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="H32" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="H32" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>41</v>
       </c>
@@ -3058,22 +3079,22 @@
         <v>4</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G33" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="H33" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="H33" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>52</v>
       </c>
@@ -3084,22 +3105,22 @@
         <v>31</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>39</v>
       </c>
@@ -3110,17 +3131,20 @@
         <v>2</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F35" s="5"/>
+      <c r="G35" s="2" t="s">
+        <v>213</v>
+      </c>
       <c r="H35" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
         <v>49</v>
       </c>
@@ -3131,20 +3155,20 @@
         <v>24</v>
       </c>
       <c r="D36" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F36" s="5"/>
       <c r="G36" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H36" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="H36" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
         <v>47</v>
       </c>
@@ -3155,20 +3179,20 @@
         <v>20</v>
       </c>
       <c r="D37" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F37" s="5"/>
       <c r="G37" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H37" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="H37" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8">
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>48</v>
       </c>
@@ -3179,20 +3203,20 @@
         <v>22</v>
       </c>
       <c r="D38" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F38" s="5"/>
       <c r="G38" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H38" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="H38" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
         <v>50</v>
       </c>
@@ -3203,20 +3227,20 @@
         <v>26</v>
       </c>
       <c r="D39" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F39" s="5"/>
       <c r="G39" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
         <v>42</v>
       </c>
@@ -3227,116 +3251,116 @@
         <v>9</v>
       </c>
       <c r="D40" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F40" s="5"/>
       <c r="G40" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H40" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="H40" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8">
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="B41" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="B41" s="13" t="s">
+      <c r="C41" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="C41" s="13" t="s">
-        <v>108</v>
-      </c>
       <c r="D41" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F41" s="5"/>
       <c r="G41" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H41" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="H41" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="C42" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="B42" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="C42" s="13" t="s">
-        <v>198</v>
-      </c>
       <c r="D42" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F42" s="5"/>
       <c r="G42" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="H42" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="H42" s="2" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B43" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="B43" s="15" t="s">
+      <c r="C43" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="C43" s="15" t="s">
-        <v>113</v>
-      </c>
       <c r="D43" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E43" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F43" s="9"/>
       <c r="G43" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="H43" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="H43" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D44" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="E44" s="11" t="s">
         <v>162</v>
-      </c>
-      <c r="B44" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="D44" s="14" t="s">
-        <v>210</v>
-      </c>
-      <c r="E44" s="11" t="s">
-        <v>163</v>
       </c>
       <c r="F44" s="11"/>
       <c r="G44" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="H44" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="H44" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>51</v>
       </c>
@@ -3347,10 +3371,10 @@
         <v>28</v>
       </c>
       <c r="D45" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E45" s="11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F45" s="11"/>
       <c r="G45" s="2" t="s">
@@ -3360,38 +3384,38 @@
         <v>91</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D46" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F46" s="11"/>
       <c r="G46" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H45">
-    <sortState ref="A2:H45">
+  <autoFilter ref="A1:H45" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H45">
       <sortCondition ref="E2:E45"/>
       <sortCondition ref="F2:F45"/>
     </sortState>
   </autoFilter>
-  <sortState ref="A2:J46">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J46">
     <sortCondition ref="E2:E46"/>
   </sortState>
   <phoneticPr fontId="7" type="noConversion"/>

</xml_diff>

<commit_message>
A few small adjustments
</commit_message>
<xml_diff>
--- a/tabular/core/hepadna-ncbi-refseqs-side-data.xlsx
+++ b/tabular/core/hepadna-ncbi-refseqs-side-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNArt/Hepadnaviridae-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6A1719A-DE29-F140-BE02-5F754ED8406C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A98C99E7-C054-1C43-866B-D03B86E630D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10340" yWindow="460" windowWidth="17340" windowHeight="14460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2256,7 +2256,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D25" workbookViewId="0">
       <selection activeCell="D12" sqref="A1:H46"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Applied correct rotation to avihepadnavirus sequences (now 85-87% genome coverage in alignment)
</commit_message>
<xml_diff>
--- a/tabular/core/hepadna-ncbi-refseqs-side-data.xlsx
+++ b/tabular/core/hepadna-ncbi-refseqs-side-data.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNArt/Hepadnaviridae-GLUE/tabular/core/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A98C99E7-C054-1C43-866B-D03B86E630D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10340" yWindow="460" windowWidth="17340" windowHeight="14460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1280" yWindow="0" windowWidth="17340" windowHeight="14460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$45</definedName>
   </definedNames>
-  <calcPr calcId="140000"/>
+  <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -678,7 +672,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2253,14 +2247,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D25" workbookViewId="0">
-      <selection activeCell="D12" sqref="A1:H46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="17.1640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" style="2" customWidth="1"/>
@@ -2272,7 +2266,7 @@
     <col min="9" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>184</v>
       </c>
@@ -2298,7 +2292,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="13" t="s">
         <v>38</v>
       </c>
@@ -2322,7 +2316,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="13" t="s">
         <v>40</v>
       </c>
@@ -2346,7 +2340,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="13" t="s">
         <v>46</v>
       </c>
@@ -2370,7 +2364,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="13" t="s">
         <v>43</v>
       </c>
@@ -2394,7 +2388,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="13" t="s">
         <v>45</v>
       </c>
@@ -2418,7 +2412,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="13" t="s">
         <v>44</v>
       </c>
@@ -2442,7 +2436,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="13" t="s">
         <v>55</v>
       </c>
@@ -2466,7 +2460,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="15" t="s">
         <v>56</v>
       </c>
@@ -2490,7 +2484,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="15" t="s">
         <v>58</v>
       </c>
@@ -2514,7 +2508,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="15" t="s">
         <v>62</v>
       </c>
@@ -2538,7 +2532,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="13" t="s">
         <v>54</v>
       </c>
@@ -2562,7 +2556,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="15" t="s">
         <v>115</v>
       </c>
@@ -2586,7 +2580,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="15" t="s">
         <v>119</v>
       </c>
@@ -2610,7 +2604,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="13" t="s">
         <v>53</v>
       </c>
@@ -2634,7 +2628,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="15" t="s">
         <v>189</v>
       </c>
@@ -2658,7 +2652,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" s="15" t="s">
         <v>122</v>
       </c>
@@ -2682,7 +2676,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" s="15" t="s">
         <v>126</v>
       </c>
@@ -2706,7 +2700,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" s="15" t="s">
         <v>129</v>
       </c>
@@ -2730,7 +2724,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" s="15" t="s">
         <v>132</v>
       </c>
@@ -2756,7 +2750,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" s="15" t="s">
         <v>135</v>
       </c>
@@ -2782,7 +2776,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22" s="15" t="s">
         <v>138</v>
       </c>
@@ -2808,7 +2802,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23" s="15" t="s">
         <v>139</v>
       </c>
@@ -2834,7 +2828,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="A24" s="15" t="s">
         <v>142</v>
       </c>
@@ -2860,7 +2854,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="A25" s="15" t="s">
         <v>145</v>
       </c>
@@ -2886,7 +2880,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="A26" s="15" t="s">
         <v>210</v>
       </c>
@@ -2912,7 +2906,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" s="15" t="s">
         <v>148</v>
       </c>
@@ -2938,7 +2932,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" s="15" t="s">
         <v>150</v>
       </c>
@@ -2964,7 +2958,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="A29" s="15" t="s">
         <v>151</v>
       </c>
@@ -2990,7 +2984,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30" s="15" t="s">
         <v>154</v>
       </c>
@@ -3016,7 +3010,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31" s="15" t="s">
         <v>157</v>
       </c>
@@ -3042,7 +3036,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32" s="15" t="s">
         <v>160</v>
       </c>
@@ -3068,7 +3062,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33" s="13" t="s">
         <v>41</v>
       </c>
@@ -3094,7 +3088,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" s="13" t="s">
         <v>52</v>
       </c>
@@ -3120,7 +3114,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35" s="13" t="s">
         <v>39</v>
       </c>
@@ -3144,7 +3138,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="A36" s="13" t="s">
         <v>49</v>
       </c>
@@ -3168,7 +3162,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37" s="13" t="s">
         <v>47</v>
       </c>
@@ -3192,7 +3186,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8">
       <c r="A38" s="13" t="s">
         <v>48</v>
       </c>
@@ -3216,7 +3210,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="A39" s="13" t="s">
         <v>50</v>
       </c>
@@ -3240,7 +3234,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="A40" s="13" t="s">
         <v>42</v>
       </c>
@@ -3264,7 +3258,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="A41" s="13" t="s">
         <v>105</v>
       </c>
@@ -3288,7 +3282,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8">
       <c r="A42" s="13" t="s">
         <v>196</v>
       </c>
@@ -3312,7 +3306,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8">
       <c r="A43" s="15" t="s">
         <v>110</v>
       </c>
@@ -3336,7 +3330,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8">
       <c r="A44" s="15" t="s">
         <v>161</v>
       </c>
@@ -3360,7 +3354,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8">
       <c r="A45" s="13" t="s">
         <v>51</v>
       </c>
@@ -3384,7 +3378,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8">
       <c r="A46" s="2" t="s">
         <v>203</v>
       </c>
@@ -3409,13 +3403,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H45" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H45">
+  <autoFilter ref="A1:H45">
+    <sortState ref="A2:H45">
       <sortCondition ref="E2:E45"/>
       <sortCondition ref="F2:F45"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J46">
+  <sortState ref="A2:J46">
     <sortCondition ref="E2:E46"/>
   </sortState>
   <phoneticPr fontId="7" type="noConversion"/>

</xml_diff>

<commit_message>
Inherit feature locations across all references
</commit_message>
<xml_diff>
--- a/tabular/core/hepadna-ncbi-refseqs-side-data.xlsx
+++ b/tabular/core/hepadna-ncbi-refseqs-side-data.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10308"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNArt/Hepadnaviridae-GLUE/tabular/core/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBAA8C06-94B9-3447-836A-D42269CB1523}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="0" windowWidth="17340" windowHeight="14460" tabRatio="500"/>
+    <workbookView xWindow="1280" yWindow="460" windowWidth="17340" windowHeight="14460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$45</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="217">
   <si>
     <t>DHBV</t>
   </si>
@@ -192,12 +198,6 @@
     <t>NC_035210</t>
   </si>
   <si>
-    <t>AY494851</t>
-  </si>
-  <si>
-    <t>Puna teal</t>
-  </si>
-  <si>
     <t>AJ441111</t>
   </si>
   <si>
@@ -222,9 +222,6 @@
     <t>Ciconia ciconia</t>
   </si>
   <si>
-    <t>Nackednavirus</t>
-  </si>
-  <si>
     <t>ACNDV</t>
   </si>
   <si>
@@ -279,9 +276,6 @@
     <t>Elegant crested tinamou</t>
   </si>
   <si>
-    <t>Spatula puna</t>
-  </si>
-  <si>
     <t>Grey crowned crane</t>
   </si>
   <si>
@@ -528,12 +522,6 @@
     <t>Skink herpetohepadnavirus</t>
   </si>
   <si>
-    <t>Astatotilapia nackednavirus</t>
-  </si>
-  <si>
-    <t>Western mosquitofish nackednavirus</t>
-  </si>
-  <si>
     <t>Spiny lizard herpetohepadnavirus</t>
   </si>
   <si>
@@ -543,33 +531,6 @@
     <t>Tetra metahepadnavirus</t>
   </si>
   <si>
-    <t>Bluefin killifish nackednavirus</t>
-  </si>
-  <si>
-    <t>Killifish nackednavirus Lp 1</t>
-  </si>
-  <si>
-    <t>Killifish nackednavirus Lp 2</t>
-  </si>
-  <si>
-    <t>European eel nackednavirus</t>
-  </si>
-  <si>
-    <t>Tiger rockfish nackednavirus</t>
-  </si>
-  <si>
-    <t>Baby whale nackednavirus</t>
-  </si>
-  <si>
-    <t>Sockeye salmon nackednavirus</t>
-  </si>
-  <si>
-    <t>Yellow drum nackednavirus</t>
-  </si>
-  <si>
-    <t>Stickleback nackednavirus</t>
-  </si>
-  <si>
     <t>Coho salmon parahepadnavirus</t>
   </si>
   <si>
@@ -667,12 +628,63 @@
   </si>
   <si>
     <t>California ground squirrel</t>
+  </si>
+  <si>
+    <t>MK620908</t>
+  </si>
+  <si>
+    <t>Tai Forest hepadnavirus</t>
+  </si>
+  <si>
+    <t>TaiHBV</t>
+  </si>
+  <si>
+    <t>Philantomba maxwellii</t>
+  </si>
+  <si>
+    <t>Maxwell's duiker</t>
+  </si>
+  <si>
+    <t>Bluefin killifish Nakednavirus</t>
+  </si>
+  <si>
+    <t>Nakednavirus</t>
+  </si>
+  <si>
+    <t>Western mosquitofish Nakednavirus</t>
+  </si>
+  <si>
+    <t>Astatotilapia Nakednavirus</t>
+  </si>
+  <si>
+    <t>Killifish Nakednavirus Lp 1</t>
+  </si>
+  <si>
+    <t>European eel Nakednavirus</t>
+  </si>
+  <si>
+    <t>Tiger rockfish Nakednavirus</t>
+  </si>
+  <si>
+    <t>Baby whale Nakednavirus</t>
+  </si>
+  <si>
+    <t>Sockeye salmon Nakednavirus</t>
+  </si>
+  <si>
+    <t>Yellow drum Nakednavirus</t>
+  </si>
+  <si>
+    <t>Stickleback Nakednavirus</t>
+  </si>
+  <si>
+    <t>Killifish Nakednavirus Lp 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2247,14 +2259,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.1640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" style="2" customWidth="1"/>
@@ -2266,33 +2278,33 @@
     <col min="9" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>38</v>
       </c>
@@ -2303,20 +2315,20 @@
         <v>1</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="2" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>40</v>
       </c>
@@ -2327,20 +2339,20 @@
         <v>3</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>46</v>
       </c>
@@ -2351,20 +2363,20 @@
         <v>19</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>43</v>
       </c>
@@ -2375,20 +2387,20 @@
         <v>12</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>45</v>
       </c>
@@ -2399,20 +2411,20 @@
         <v>16</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>44</v>
       </c>
@@ -2423,20 +2435,20 @@
         <v>15</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="2" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>55</v>
       </c>
@@ -2447,212 +2459,212 @@
         <v>34</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>56</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>1</v>
+        <v>58</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="2" t="s">
-        <v>85</v>
+        <v>59</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>64</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>209</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="7"/>
+        <v>194</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="F11" s="10"/>
       <c r="G11" s="2" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>33</v>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>164</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="F12" s="10"/>
       <c r="G12" s="2" t="s">
-        <v>72</v>
+        <v>113</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>115</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>170</v>
+      <c r="C13" s="15" t="s">
+        <v>163</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="H13" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="15" t="s">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="F14" s="4"/>
+      <c r="G14" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>119</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>167</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>209</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="F14" s="10"/>
-      <c r="G14" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>209</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>123</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="2" t="s">
-        <v>88</v>
+        <v>177</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>189</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>202</v>
+        <v>118</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>165</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="2" t="s">
-        <v>192</v>
+        <v>120</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>122</v>
       </c>
@@ -2660,701 +2672,701 @@
         <v>122</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="H17" s="2" t="s">
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="15" t="s">
-        <v>126</v>
-      </c>
       <c r="B18" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="H18" s="2" t="s">
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="15" t="s">
+      <c r="B19" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B19" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>166</v>
-      </c>
-      <c r="D19" s="14" t="s">
+      <c r="H19" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="C22" s="15" t="s">
         <v>209</v>
       </c>
-      <c r="E19" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="F19" s="4"/>
-      <c r="G19" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>209</v>
-      </c>
-      <c r="E20" s="12" t="s">
+      <c r="D22" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="G25" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="F20" s="12" t="s">
-        <v>193</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>169</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>209</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>193</v>
-      </c>
-      <c r="G21" s="2" t="s">
+      <c r="H25" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="F27" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="F29" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="F30" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="F31" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="G31" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="H31" s="2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="D22" s="14" t="s">
-        <v>209</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>193</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="D23" s="14" t="s">
-        <v>209</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="F23" s="12" t="s">
-        <v>193</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>176</v>
-      </c>
-      <c r="D24" s="14" t="s">
-        <v>209</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="F24" s="12" t="s">
-        <v>193</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>177</v>
-      </c>
-      <c r="D25" s="14" t="s">
-        <v>209</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="F25" s="12" t="s">
-        <v>193</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="15" t="s">
-        <v>210</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="C26" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="D26" s="14" t="s">
-        <v>209</v>
-      </c>
-      <c r="E26" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="F26" s="12" t="s">
-        <v>193</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="H26" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>178</v>
-      </c>
-      <c r="D27" s="14" t="s">
-        <v>209</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="F27" s="16" t="s">
-        <v>194</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="15" t="s">
-        <v>150</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>150</v>
-      </c>
-      <c r="C28" s="15" t="s">
-        <v>178</v>
-      </c>
-      <c r="D28" s="14" t="s">
-        <v>209</v>
-      </c>
-      <c r="E28" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="F28" s="16" t="s">
-        <v>194</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="C29" s="15" t="s">
-        <v>179</v>
-      </c>
-      <c r="D29" s="14" t="s">
-        <v>209</v>
-      </c>
-      <c r="E29" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="F29" s="16" t="s">
-        <v>194</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="C30" s="15" t="s">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="D30" s="14" t="s">
-        <v>209</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="F30" s="16" t="s">
-        <v>194</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="C31" s="15" t="s">
-        <v>181</v>
-      </c>
-      <c r="D31" s="14" t="s">
-        <v>209</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="F31" s="16" t="s">
-        <v>194</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="A32" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="C32" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="D32" s="14" t="s">
-        <v>209</v>
-      </c>
-      <c r="E32" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="F32" s="16" t="s">
-        <v>194</v>
-      </c>
       <c r="G32" s="2" t="s">
-        <v>140</v>
+        <v>89</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>93</v>
+        <v>186</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F34" s="5" t="s">
-        <v>195</v>
-      </c>
+      <c r="F34" s="5"/>
       <c r="G34" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F35" s="5"/>
       <c r="G35" s="2" t="s">
-        <v>213</v>
+        <v>91</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D36" s="14" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F36" s="5"/>
       <c r="G36" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D37" s="14" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F37" s="5"/>
       <c r="G37" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D38" s="14" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F38" s="5"/>
       <c r="G38" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="D39" s="14" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F39" s="5"/>
       <c r="G39" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H39" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="H39" s="2" t="s">
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="13" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="40" spans="1:8">
-      <c r="A40" s="13" t="s">
-        <v>42</v>
-      </c>
       <c r="B40" s="13" t="s">
-        <v>8</v>
+        <v>102</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>9</v>
+        <v>103</v>
       </c>
       <c r="D40" s="14" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F40" s="5"/>
       <c r="G40" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
-        <v>105</v>
+        <v>181</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>106</v>
+        <v>185</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>107</v>
+        <v>182</v>
       </c>
       <c r="D41" s="14" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F41" s="5"/>
       <c r="G41" s="2" t="s">
-        <v>108</v>
+        <v>183</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="D42" s="14" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F42" s="5"/>
       <c r="G42" s="2" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="15" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D43" s="14" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="E43" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F43" s="9"/>
       <c r="G43" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="15" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B44" s="15" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="D44" s="14" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="E44" s="11" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="F44" s="11"/>
       <c r="G44" s="2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>51</v>
       </c>
@@ -3365,51 +3377,51 @@
         <v>28</v>
       </c>
       <c r="D45" s="14" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="E45" s="11" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="F45" s="11"/>
       <c r="G45" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="D46" s="14" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="F46" s="11"/>
       <c r="G46" s="2" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H45">
-    <sortState ref="A2:H45">
+  <autoFilter ref="A1:H45" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H45">
       <sortCondition ref="E2:E45"/>
       <sortCondition ref="F2:F45"/>
     </sortState>
   </autoFilter>
-  <sortState ref="A2:J46">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J46">
     <sortCondition ref="E2:E46"/>
   </sortState>
   <phoneticPr fontId="7" type="noConversion"/>

</xml_diff>

<commit_message>
Update ehbv alignments and references
</commit_message>
<xml_diff>
--- a/tabular/core/hepadna-ncbi-refseqs-side-data.xlsx
+++ b/tabular/core/hepadna-ncbi-refseqs-side-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNArt/Hepadnaviridae-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBAA8C06-94B9-3447-836A-D42269CB1523}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64DDD0A-F0AC-BF48-9E74-43BC70C399D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1280" yWindow="460" windowWidth="17340" windowHeight="14460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2262,8 +2262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added more locus information (in line with template set in AAV-GLUE)
</commit_message>
<xml_diff>
--- a/tabular/core/hepadna-ncbi-refseqs-side-data.xlsx
+++ b/tabular/core/hepadna-ncbi-refseqs-side-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNArt/Hepadnaviridae-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64DDD0A-F0AC-BF48-9E74-43BC70C399D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43971C5C-1D16-DD49-9EAE-C4203D7BAE1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1280" yWindow="460" windowWidth="17340" windowHeight="14460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2262,8 +2262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26:D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Refactoring. Categorisation of variable regions - data exported for figtree annotation
</commit_message>
<xml_diff>
--- a/tabular/core/hepadna-ncbi-refseqs-side-data.xlsx
+++ b/tabular/core/hepadna-ncbi-refseqs-side-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNArt/Hepadnaviridae-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D85C85C-0FF0-1A47-BEE2-37A6B23E37D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C76EAA-D656-2D42-8F12-9D851DADCF39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="460" windowWidth="27960" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-1180" yWindow="460" windowWidth="27340" windowHeight="16160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="237">
   <si>
     <t>DHBV</t>
   </si>
@@ -680,6 +680,66 @@
   </si>
   <si>
     <t>Killifish Nakednavirus Lp 2</t>
+  </si>
+  <si>
+    <t>core_shift</t>
+  </si>
+  <si>
+    <t>type-2</t>
+  </si>
+  <si>
+    <t>type-1</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>variable_region_type</t>
+  </si>
+  <si>
+    <t>avi-1-modern</t>
+  </si>
+  <si>
+    <t>ortho-type-1</t>
+  </si>
+  <si>
+    <t>ortho-type-2</t>
+  </si>
+  <si>
+    <t>ortho-type-6</t>
+  </si>
+  <si>
+    <t>ortho-type-2a</t>
+  </si>
+  <si>
+    <t>ortho-type 4</t>
+  </si>
+  <si>
+    <t>ortho-type 5</t>
+  </si>
+  <si>
+    <t>ortho-type 3</t>
+  </si>
+  <si>
+    <t>meta-type-3</t>
+  </si>
+  <si>
+    <t>meta-type-1</t>
+  </si>
+  <si>
+    <t>meta-type-4</t>
+  </si>
+  <si>
+    <t>meta-type-2</t>
+  </si>
+  <si>
+    <t>ND</t>
+  </si>
+  <si>
+    <t>herpeto-type-1</t>
+  </si>
+  <si>
+    <t>herpeto-type-2</t>
   </si>
 </sst>
 </file>
@@ -746,7 +806,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -807,6 +867,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14996795556505021"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1362,7 +1440,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1371,7 +1449,6 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1380,6 +1457,9 @@
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="543">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2261,10 +2341,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2276,10 +2356,12 @@
     <col min="5" max="6" width="23.5" style="2" customWidth="1"/>
     <col min="7" max="7" width="28.5" style="2" customWidth="1"/>
     <col min="8" max="8" width="25.83203125" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="2"/>
+    <col min="9" max="9" width="30" style="2" customWidth="1"/>
+    <col min="10" max="10" width="24.5" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>169</v>
       </c>
@@ -2304,426 +2386,534 @@
       <c r="H1" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="I1" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="13" t="s">
         <v>194</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F2" s="3"/>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="12" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="I2" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="13" t="s">
         <v>194</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F3" s="3"/>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="12" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="I3" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="13" t="s">
         <v>194</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="3"/>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="12" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="I4" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="13" t="s">
         <v>194</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="3"/>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="12" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="I5" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="13" t="s">
         <v>194</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F6" s="3"/>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="12" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="I6" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="13" t="s">
         <v>194</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="3"/>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="12" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="I7" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="13" t="s">
         <v>194</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F8" s="3"/>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="12" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="I8" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="13" t="s">
         <v>194</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F9" s="7"/>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="12" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="I9" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="13" t="s">
         <v>194</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F10" s="7"/>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="12" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+      <c r="I10" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="14" t="s">
-        <v>194</v>
-      </c>
-      <c r="E11" s="10" t="s">
+      <c r="D11" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="E11" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="F11" s="10"/>
-      <c r="G11" s="2" t="s">
+      <c r="F11" s="9"/>
+      <c r="G11" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="12" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
+      <c r="I11" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="14" t="s">
         <v>111</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="D12" s="14" t="s">
-        <v>194</v>
-      </c>
-      <c r="E12" s="10" t="s">
+      <c r="D12" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="E12" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="F12" s="10"/>
-      <c r="G12" s="2" t="s">
+      <c r="F12" s="9"/>
+      <c r="G12" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="12" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
+      <c r="I12" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="14" t="s">
         <v>163</v>
       </c>
-      <c r="D13" s="14" t="s">
-        <v>194</v>
-      </c>
-      <c r="E13" s="10" t="s">
+      <c r="D13" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="E13" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="F13" s="10"/>
-      <c r="G13" s="2" t="s">
+      <c r="F13" s="9"/>
+      <c r="G13" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H13" s="12" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="I13" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="13" t="s">
         <v>194</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>119</v>
       </c>
       <c r="F14" s="4"/>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="12" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
+      <c r="I14" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="12" t="s">
         <v>187</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="13" t="s">
         <v>194</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>119</v>
       </c>
       <c r="F15" s="4"/>
-      <c r="G15" s="2" t="s">
+      <c r="G15" s="12" t="s">
         <v>177</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H15" s="12" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
+      <c r="I15" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="13" t="s">
         <v>194</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>119</v>
       </c>
       <c r="F16" s="4"/>
-      <c r="G16" s="2" t="s">
+      <c r="G16" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H16" s="12" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
+      <c r="I16" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="13" t="s">
         <v>194</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>119</v>
       </c>
       <c r="F17" s="4"/>
-      <c r="G17" s="2" t="s">
+      <c r="G17" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="H17" s="12" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
+      <c r="I17" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="13" t="s">
         <v>194</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>119</v>
       </c>
       <c r="F18" s="4"/>
-      <c r="G18" s="2" t="s">
+      <c r="G18" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="H18" s="12" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
+      <c r="I18" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D19" s="13" t="s">
         <v>194</v>
       </c>
       <c r="E19" s="5" t="s">
@@ -2732,24 +2922,30 @@
       <c r="F19" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="G19" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="H19" s="12" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
+      <c r="I19" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="13" t="s">
         <v>194</v>
       </c>
       <c r="E20" s="5" t="s">
@@ -2758,302 +2954,380 @@
       <c r="F20" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G20" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="H20" s="12" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
+      <c r="I20" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="13" t="s">
         <v>194</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F21" s="5"/>
-      <c r="G21" s="2" t="s">
+      <c r="G21" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="H21" s="12" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
+      <c r="I21" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="14" t="s">
+      <c r="D22" s="13" t="s">
         <v>194</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F22" s="5"/>
-      <c r="G22" s="2" t="s">
+      <c r="G22" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="H22" s="12" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
+      <c r="I22" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="D23" s="13" t="s">
         <v>194</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F23" s="5"/>
-      <c r="G23" s="2" t="s">
+      <c r="G23" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="H23" s="12" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
+      <c r="I23" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="14" t="s">
+      <c r="D24" s="13" t="s">
         <v>194</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F24" s="5"/>
-      <c r="G24" s="2" t="s">
+      <c r="G24" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="H24" s="2" t="s">
+      <c r="H24" s="12" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
+      <c r="I24" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="D25" s="13" t="s">
         <v>194</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F25" s="5"/>
-      <c r="G25" s="2" t="s">
+      <c r="G25" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="H25" s="2" t="s">
+      <c r="H25" s="12" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
+      <c r="I25" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="D26" s="13" t="s">
         <v>194</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F26" s="5"/>
-      <c r="G26" s="2" t="s">
+      <c r="G26" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="H26" s="12" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="s">
+      <c r="I26" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D27" s="13" t="s">
         <v>194</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F27" s="5"/>
-      <c r="G27" s="2" t="s">
+      <c r="G27" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="H27" s="2" t="s">
+      <c r="H27" s="12" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="s">
+      <c r="I27" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
         <v>181</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="D28" s="13" t="s">
         <v>194</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F28" s="5"/>
-      <c r="G28" s="2" t="s">
+      <c r="G28" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="H28" s="2" t="s">
+      <c r="H28" s="12" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="s">
+      <c r="I28" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
         <v>200</v>
       </c>
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="12" t="s">
         <v>201</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="D29" s="13" t="s">
         <v>194</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F29" s="5"/>
-      <c r="G29" s="2" t="s">
+      <c r="G29" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="H29" s="2" t="s">
+      <c r="H29" s="12" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="15" t="s">
+      <c r="I29" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="C30" s="15" t="s">
+      <c r="C30" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="D30" s="14" t="s">
-        <v>194</v>
-      </c>
-      <c r="E30" s="9" t="s">
+      <c r="D30" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="E30" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F30" s="9"/>
-      <c r="G30" s="2" t="s">
+      <c r="F30" s="8"/>
+      <c r="G30" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="H30" s="2" t="s">
+      <c r="H30" s="12" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="15" t="s">
+      <c r="I30" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="J30" s="5" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="14" t="s">
         <v>157</v>
       </c>
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="14" t="s">
         <v>157</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="D31" s="14" t="s">
-        <v>194</v>
-      </c>
-      <c r="E31" s="11" t="s">
+      <c r="D31" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="E31" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="F31" s="11"/>
-      <c r="G31" s="2" t="s">
+      <c r="F31" s="10"/>
+      <c r="G31" s="12" t="s">
         <v>159</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="H31" s="12" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="s">
+      <c r="I31" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="J31" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="B32" s="13" t="s">
+      <c r="B32" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D32" s="14" t="s">
-        <v>194</v>
-      </c>
-      <c r="E32" s="11" t="s">
+      <c r="D32" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="E32" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="F32" s="11"/>
-      <c r="G32" s="2" t="s">
+      <c r="F32" s="10"/>
+      <c r="G32" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="H32" s="2" t="s">
+      <c r="H32" s="12" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="J32" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>188</v>
       </c>
@@ -3063,18 +3337,24 @@
       <c r="C33" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="D33" s="14" t="s">
-        <v>194</v>
-      </c>
-      <c r="E33" s="11" t="s">
+      <c r="D33" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="E33" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="F33" s="11"/>
-      <c r="G33" s="2" t="s">
+      <c r="F33" s="10"/>
+      <c r="G33" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="H33" s="2" t="s">
+      <c r="H33" s="12" t="s">
         <v>189</v>
+      </c>
+      <c r="I33" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="J33" s="10" t="s">
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -3108,23 +3388,23 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>128</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="D1" s="14" t="s">
-        <v>194</v>
-      </c>
-      <c r="E1" s="12" t="s">
+      <c r="D1" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>178</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -3134,23 +3414,23 @@
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:8" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="14" t="s">
         <v>207</v>
       </c>
-      <c r="D2" s="14" t="s">
-        <v>194</v>
-      </c>
-      <c r="E2" s="12" t="s">
+      <c r="D2" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="11" t="s">
         <v>178</v>
       </c>
       <c r="G2" s="2" t="s">
@@ -3160,23 +3440,23 @@
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+    <row r="3" spans="1:8" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="14" t="s">
         <v>208</v>
       </c>
-      <c r="D3" s="14" t="s">
-        <v>194</v>
-      </c>
-      <c r="E3" s="12" t="s">
+      <c r="D3" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="E3" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="11" t="s">
         <v>178</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -3186,23 +3466,23 @@
         <v>121</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+    <row r="4" spans="1:8" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="14" t="s">
         <v>209</v>
       </c>
-      <c r="D4" s="14" t="s">
-        <v>194</v>
-      </c>
-      <c r="E4" s="12" t="s">
+      <c r="D4" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="11" t="s">
         <v>178</v>
       </c>
       <c r="G4" s="2" t="s">
@@ -3212,23 +3492,23 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+    <row r="5" spans="1:8" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="14" t="s">
         <v>210</v>
       </c>
-      <c r="D5" s="14" t="s">
-        <v>194</v>
-      </c>
-      <c r="E5" s="12" t="s">
+      <c r="D5" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="11" t="s">
         <v>178</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -3238,23 +3518,23 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+    <row r="6" spans="1:8" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="14" t="s">
         <v>211</v>
       </c>
-      <c r="D6" s="14" t="s">
-        <v>194</v>
-      </c>
-      <c r="E6" s="12" t="s">
+      <c r="D6" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="E6" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="11" t="s">
         <v>178</v>
       </c>
       <c r="G6" s="2" t="s">
@@ -3264,23 +3544,23 @@
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+    <row r="7" spans="1:8" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="D7" s="14" t="s">
-        <v>194</v>
-      </c>
-      <c r="E7" s="12" t="s">
+      <c r="D7" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="E7" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="11" t="s">
         <v>178</v>
       </c>
       <c r="G7" s="2" t="s">
@@ -3290,23 +3570,23 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+    <row r="8" spans="1:8" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="14" t="s">
         <v>212</v>
       </c>
-      <c r="D8" s="14" t="s">
-        <v>194</v>
-      </c>
-      <c r="E8" s="12" t="s">
+      <c r="D8" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="E8" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F8" s="15" t="s">
         <v>179</v>
       </c>
       <c r="G8" s="2" t="s">
@@ -3316,23 +3596,23 @@
         <v>161</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+    <row r="9" spans="1:8" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="14" t="s">
         <v>212</v>
       </c>
-      <c r="D9" s="14" t="s">
-        <v>194</v>
-      </c>
-      <c r="E9" s="12" t="s">
+      <c r="D9" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="E9" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="15" t="s">
         <v>179</v>
       </c>
       <c r="G9" s="2" t="s">
@@ -3342,23 +3622,23 @@
         <v>161</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+    <row r="10" spans="1:8" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="14" t="s">
         <v>213</v>
       </c>
-      <c r="D10" s="14" t="s">
-        <v>194</v>
-      </c>
-      <c r="E10" s="12" t="s">
+      <c r="D10" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="E10" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="F10" s="15" t="s">
         <v>179</v>
       </c>
       <c r="G10" s="2" t="s">
@@ -3368,23 +3648,23 @@
         <v>149</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
+    <row r="11" spans="1:8" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="14" t="s">
         <v>214</v>
       </c>
-      <c r="D11" s="14" t="s">
-        <v>194</v>
-      </c>
-      <c r="E11" s="12" t="s">
+      <c r="D11" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="E11" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="15" t="s">
         <v>179</v>
       </c>
       <c r="G11" s="2" t="s">
@@ -3394,23 +3674,23 @@
         <v>152</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
+    <row r="12" spans="1:8" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="14" t="s">
         <v>215</v>
       </c>
-      <c r="D12" s="14" t="s">
-        <v>194</v>
-      </c>
-      <c r="E12" s="12" t="s">
+      <c r="D12" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="E12" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="F12" s="15" t="s">
         <v>179</v>
       </c>
       <c r="G12" s="2" t="s">
@@ -3420,23 +3700,23 @@
         <v>155</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
+    <row r="13" spans="1:8" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
         <v>156</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="14" t="s">
         <v>156</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="14" t="s">
         <v>216</v>
       </c>
-      <c r="D13" s="14" t="s">
-        <v>194</v>
-      </c>
-      <c r="E13" s="12" t="s">
+      <c r="D13" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="E13" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="15" t="s">
         <v>179</v>
       </c>
       <c r="G13" s="2" t="s">

</xml_diff>

<commit_message>
Refactor eHBV names and alignments
</commit_message>
<xml_diff>
--- a/tabular/core/hepadna-ncbi-refseqs-side-data.xlsx
+++ b/tabular/core/hepadna-ncbi-refseqs-side-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNArt/Hepadnaviridae-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C76EAA-D656-2D42-8F12-9D851DADCF39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B865E0BD-473B-734E-9E2D-EC5E6865548B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1180" yWindow="460" windowWidth="27340" windowHeight="16160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="840" yWindow="460" windowWidth="27340" windowHeight="16160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2343,8 +2343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Refactoring - inclusion of recently identified Orthohepadnaviruses
</commit_message>
<xml_diff>
--- a/tabular/core/hepadna-ncbi-refseqs-side-data.xlsx
+++ b/tabular/core/hepadna-ncbi-refseqs-side-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10509"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNArt/Hepadnaviridae-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BD1DCE5-E367-F844-989D-A62F6C85688E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB7782D-F4C1-A247-8A8B-9851B18085DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="500" windowWidth="27340" windowHeight="16160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8300" yWindow="1900" windowWidth="31460" windowHeight="21500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2361,8 +2361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="J34" sqref="A1:J34"/>
+    <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>

</xml_diff>